<commit_message>
improve support of large numbers
</commit_message>
<xml_diff>
--- a/src/test/resources/many_data.xlsx
+++ b/src/test/resources/many_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Xavier</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>NumberAsString</t>
   </si>
 </sst>
 </file>
@@ -142,11 +145,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,12 +172,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="14">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -500,19 +515,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="7.83203125" customWidth="1"/>
     <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -543,8 +559,11 @@
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -577,15 +596,18 @@
       <c r="J2" s="5">
         <v>0.2</v>
       </c>
+      <c r="K2">
+        <v>123</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -618,8 +640,11 @@
       <c r="J4" s="5">
         <v>0.05</v>
       </c>
+      <c r="K4">
+        <v>1234567890</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -651,6 +676,9 @@
       </c>
       <c r="J5" s="5">
         <v>0.6</v>
+      </c>
+      <c r="K5">
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>